<commit_message>
updates to axe swing
</commit_message>
<xml_diff>
--- a/plans/BeginnerBouldering.xlsx
+++ b/plans/BeginnerBouldering.xlsx
@@ -700,7 +700,7 @@
         <rFont val="Arial"/>
         <b val="0"/>
       </rPr>
-      <t xml:space="preserve">Stand sideways to a high cable machine with feet shoulder-width apart. Hold the handle with both hands above your left shoulder. Pull the cable down and across your body to your right hip in a chopping motion, rotating through your torso while keeping your hips stable. Focus on engaging your core and obliques—like a controlled twist you'd use when flagging or twisting into a reach. Slowly return and repeat. Great for building rotational strength and body tension for climbing moves.
+      <t xml:space="preserve">Stand sideways to a high cable machine with feet shoulder-width apart. Hold the handle with both hands above your left shoulder. Pull the cable across your body to your right while keeping your arms straight rotating through your torso while keeping your hips stable. Focus on engaging your core and obliques—like a controlled twist you'd use when flagging or twisting into a reach. Slowly return and repeat. Great for building rotational strength and body tension for climbing moves.
 </t>
     </r>
     <r>
@@ -1334,7 +1334,7 @@
         <rFont val="Arial"/>
         <b val="0"/>
       </rPr>
-      <t xml:space="preserve">Stand sideways to a high cable machine with feet shoulder-width apart. Hold the handle with both hands above your left shoulder. Pull the cable down and across your body to your right hip in a chopping motion, rotating through your torso while keeping your hips stable. Focus on engaging your core and obliques—like a controlled twist you'd use when flagging or twisting into a reach. Slowly return and repeat. Great for building rotational strength and body tension for climbing moves.
+      <t xml:space="preserve">Stand sideways to a high cable machine with feet shoulder-width apart. Hold the handle with both hands above your left shoulder. Pull the cable across your body to your right while keeping your arms straight rotating through your torso while keeping your hips stable. Focus on engaging your core and obliques—like a controlled twist you'd use when flagging or twisting into a reach. Slowly return and repeat. Great for building rotational strength and body tension for climbing moves.
 </t>
     </r>
     <r>

</xml_diff>